<commit_message>
add bg music, sfx, change minigame assets
</commit_message>
<xml_diff>
--- a/Assets/Spreadsheet/Scripts/Chapter5.xlsx
+++ b/Assets/Spreadsheet/Scripts/Chapter5.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">
 @set "game_chapter = 6"
 @set "loc2_open = true"
-@choice {0} goto:.o_item set:item_owner="o" do:"@purgeRollback"
+@choice {0} goto:.o_item set:item_owner="o" do:@purgeRollback
 </t>
   </si>
   <si>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">" Віддати качку Оліверу"</t>
   </si>
   <si>
-    <t xml:space="preserve">@choice {0} goto:.j_item set:item_owner="j" do:"@purgeRollback"
+    <t xml:space="preserve">@choice {0} goto:.j_item set:item_owner="j" do:@purgeRollback
 </t>
   </si>
   <si>
@@ -114,20 +114,21 @@
     <t xml:space="preserve">" Віддати качку Джошу"</t>
   </si>
   <si>
-    <t xml:space="preserve">@choice {0} goto:.p_item set:item_owner="p" do:"@purgeRollback"
+    <t xml:space="preserve">@choice {0} goto:.p_item set:item_owner="p" do:@purgeRollback
 </t>
   </si>
   <si>
     <t xml:space="preserve">"Take duck by you self"</t>
   </si>
   <si>
-    <t xml:space="preserve">" Взяти качку собі"</t>
+    <t xml:space="preserve">"Взяти качку собі"</t>
   </si>
   <si>
     <t xml:space="preserve">@stop
 # o_item
 @char j.Stupid
 @spawn ShakeCharacter params:j
+@set "game_chapter = 7"
 o: {0}
 </t>
   </si>
@@ -145,11 +146,11 @@
   </si>
   <si>
     <t xml:space="preserve">
-@set "game_chapter = 7"
 @goto Map
 # j_item
 @char o.Stupid
 @spawn ShakeCharacter params:o
+@set "game_chapter = 7"
 j: {0}
 </t>
   </si>
@@ -171,13 +172,13 @@
   </si>
   <si>
     <t xml:space="preserve">
-@set "game_chapter = 7"
 @goto Map
 # p_item
 @char o.Stupid
 @char j.Stupid
 @spawn ShakeCharacter params:o
 @spawn ShakeCharacter params:j
+@set "game_chapter = 7"
 o.Stupid: {0}
 </t>
   </si>
@@ -199,7 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-@set "game_chapter = 7"
 @goto Map</t>
   </si>
 </sst>
@@ -303,7 +303,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,7 +346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -357,7 +357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -368,7 +368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -456,7 +456,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -467,7 +467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>